<commit_message>
Fix: Put a mutex in the prime counter
</commit_message>
<xml_diff>
--- a/Métricas.xlsx
+++ b/Métricas.xlsx
@@ -9,9 +9,6 @@
   </bookViews>
   <sheets>
     <sheet name="Dados gerais" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Tempo" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Aceleração" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Eficiência" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,21 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t xml:space="preserve">Threads</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MédiaTempo(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aceleração</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eficiência</t>
   </si>
   <si>
     <t xml:space="preserve">N=10</t>
@@ -57,6 +42,12 @@
   <si>
     <t xml:space="preserve">N=1000000</t>
   </si>
+  <si>
+    <t xml:space="preserve">Aceleração</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eficiência</t>
+  </si>
 </sst>
 </file>
 
@@ -65,7 +56,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -87,11 +78,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -100,12 +86,6 @@
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,21 +130,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -229,7 +201,7 @@
       <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF579D1C"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF314004"/>
+      <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
@@ -259,7 +231,7 @@
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>Números X Tempo</a:t>
+              <a:t>Threads X Tempo</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -283,11 +255,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tempo!$A$2</c:f>
+              <c:f>'Dados gerais'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>N=10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -328,53 +300,35 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tempo!$B$1:$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>N=10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>N=100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>N=1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>N=10000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>N=100000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>N=100000</c:v>
+              <c:f>'Dados gerais'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tempo!$B$2:$G$2</c:f>
+              <c:f>'Dados gerais'!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.00063971</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.00075223</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.00168294</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.01118532</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.06259119</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.53035014</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.00072044</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00057068</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0005289</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -385,11 +339,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tempo!$A$3</c:f>
+              <c:f>'Dados gerais'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>N=100</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -430,53 +384,35 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tempo!$B$1:$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>N=10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>N=100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>N=1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>N=10000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>N=100000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>N=100000</c:v>
+              <c:f>'Dados gerais'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tempo!$B$3:$G$3</c:f>
+              <c:f>'Dados gerais'!$C$2:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.00059671</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.00064081</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.00107316</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.00733196</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0389873</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.28831734</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.00067737</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00057719</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00047626</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -487,11 +423,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tempo!$A$4</c:f>
+              <c:f>'Dados gerais'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>N=1000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -532,53 +468,287 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tempo!$B$1:$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>N=10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>N=100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>N=1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>N=10000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>N=100000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>N=100000</c:v>
+              <c:f>'Dados gerais'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tempo!$B$4:$G$4</c:f>
+              <c:f>'Dados gerais'!$D$2:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0.00053342</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.00056376</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.00067451</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.003302</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.02230055</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.16035245</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.00203937</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00100679</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00060595</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Dados gerais'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N=10000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="579d1c"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Dados gerais'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Dados gerais'!$E$2:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.01197194</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00694014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00245745</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Dados gerais'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N=100000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7e0021"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Dados gerais'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Dados gerais'!$F$2:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.06476401</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.03981932</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01868315</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Dados gerais'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N=1000000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="83caff"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Dados gerais'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Dados gerais'!$G$2:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.5710533</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33275941</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19386472</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -586,11 +756,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="58303143"/>
-        <c:axId val="96039438"/>
+        <c:axId val="71560624"/>
+        <c:axId val="34231772"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58303143"/>
+        <c:axId val="71560624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -611,7 +781,7 @@
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Quantidade</a:t>
+                  <a:t>Threads</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -646,7 +816,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96039438"/>
+        <c:crossAx val="34231772"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -654,7 +824,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96039438"/>
+        <c:axId val="34231772"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -719,7 +889,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58303143"/>
+        <c:crossAx val="71560624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -811,11 +981,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Aceleração!$A$1</c:f>
+              <c:f>'Dados gerais'!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Threads</c:v>
+                  <c:v>N=10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -854,9 +1024,26 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Dados gerais'!$A$7:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aceleração!$A$2:$A$4</c:f>
+              <c:f>'Dados gerais'!$B$7:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -864,10 +1051,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>1.26242377514544</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.36214785403668</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -878,11 +1065,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Aceleração!$B$1</c:f>
+              <c:f>'Dados gerais'!$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>N=10</c:v>
+                  <c:v>N=100</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -921,9 +1108,26 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Dados gerais'!$A$7:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aceleração!$B$2:$B$4</c:f>
+              <c:f>'Dados gerais'!$C$7:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -931,10 +1135,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.072061806</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.19926137</c:v>
+                  <c:v>1.17356503057919</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.42226934867509</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -945,11 +1149,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Aceleração!$C$1</c:f>
+              <c:f>'Dados gerais'!$D$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>N=100</c:v>
+                  <c:v>N=1000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -988,9 +1192,26 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Dados gerais'!$A$7:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aceleração!$C$2:$C$4</c:f>
+              <c:f>'Dados gerais'!$D$7:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -998,10 +1219,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.173873691</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.334308926</c:v>
+                  <c:v>2.02561606690571</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.36557471738592</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1012,11 +1233,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Aceleração!$D$1</c:f>
+              <c:f>'Dados gerais'!$E$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>N=1000</c:v>
+                  <c:v>N=10000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1055,9 +1276,26 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Dados gerais'!$A$7:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aceleração!$D$2:$D$4</c:f>
+              <c:f>'Dados gerais'!$E$7:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1065,10 +1303,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.568209773</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.49505567</c:v>
+                  <c:v>1.7250286017285</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.87169220126554</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1079,11 +1317,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Aceleração!$E$1</c:f>
+              <c:f>'Dados gerais'!$F$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>N=10000</c:v>
+                  <c:v>N=100000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1122,9 +1360,26 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Dados gerais'!$A$7:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aceleração!$E$2:$E$4</c:f>
+              <c:f>'Dados gerais'!$F$7:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1132,10 +1387,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.525556604</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.387437916</c:v>
+                  <c:v>1.62644691069561</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.46643954579394</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1146,11 +1401,11 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Aceleração!$F$1</c:f>
+              <c:f>'Dados gerais'!$G$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>N=100000</c:v>
+                  <c:v>N=1000000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1189,9 +1444,26 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Dados gerais'!$A$7:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aceleração!$F$2:$F$4</c:f>
+              <c:f>'Dados gerais'!$G$7:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1199,77 +1471,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6054251</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.806710597</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Aceleração!$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>N=1000000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="314004"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>Aceleração!$G$2:$G$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.839466679</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.307402787</c:v>
+                  <c:v>1.71611465472907</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.94562775527182</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1277,11 +1482,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="29808942"/>
-        <c:axId val="27558552"/>
+        <c:axId val="39911192"/>
+        <c:axId val="63862364"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="29808942"/>
+        <c:axId val="39911192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1337,7 +1542,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27558552"/>
+        <c:crossAx val="63862364"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1345,7 +1550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="27558552"/>
+        <c:axId val="63862364"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1410,7 +1615,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29808942"/>
+        <c:crossAx val="39911192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1502,7 +1707,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Eficiência!$B$1</c:f>
+              <c:f>'Dados gerais'!$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1547,7 +1752,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Eficiência!$A$2:$A$4</c:f>
+              <c:f>'Dados gerais'!$A$12:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1564,18 +1769,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Eficiência!$B$2:$B$4</c:f>
+              <c:f>'Dados gerais'!$B$12:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1563.20832877398</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1796.62114857668</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2248.24972822048</c:v>
+                  <c:v>1388.04064182999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2212.13950926165</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2575.43553419679</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1586,7 +1791,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Eficiência!$C$1</c:f>
+              <c:f>'Dados gerais'!$C$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1631,7 +1836,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Eficiência!$A$2:$A$4</c:f>
+              <c:f>'Dados gerais'!$A$12:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1648,18 +1853,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Eficiência!$C$2:$C$4</c:f>
+              <c:f>'Dados gerais'!$C$12:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1329.3806415591</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1831.8591955645</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2366.80311796513</c:v>
+                  <c:v>1476.29803504732</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2033.23867457715</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2986.32962809199</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1670,7 +1875,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Eficiência!$D$1</c:f>
+              <c:f>'Dados gerais'!$D$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1715,7 +1920,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Eficiência!$A$2:$A$4</c:f>
+              <c:f>'Dados gerais'!$A$12:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1732,18 +1937,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Eficiência!$D$2:$D$4</c:f>
+              <c:f>'Dados gerais'!$D$12:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>594.198248303564</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1461.30099240264</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3699.06401690406</c:v>
+                  <c:v>490.347509279827</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011.95489318101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5554.21192736352</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1754,7 +1959,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Eficiência!$E$1</c:f>
+              <c:f>'Dados gerais'!$E$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1799,7 +2004,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Eficiência!$A$2:$A$4</c:f>
+              <c:f>'Dados gerais'!$A$12:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1816,18 +2021,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Eficiência!$E$2:$E$4</c:f>
+              <c:f>'Dados gerais'!$E$12:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>89.4028959386052</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>208.069411758492</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1025.87459612789</c:v>
+                  <c:v>83.5286511626353</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>248.558184954265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1982.41762854404</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1838,7 +2043,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Eficiência!$F$1</c:f>
+              <c:f>'Dados gerais'!$F$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1883,7 +2088,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Eficiência!$A$2:$A$4</c:f>
+              <c:f>'Dados gerais'!$A$12:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1900,18 +2105,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Eficiência!$F$2:$F$4</c:f>
+              <c:f>'Dados gerais'!$F$12:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15.9766893711399</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41.1781554498119</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>125.858357611083</c:v>
+                  <c:v>15.4406745351315</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.8456726708445</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>185.538281595659</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1922,11 +2127,11 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Eficiência!$G$1</c:f>
+              <c:f>'Dados gerais'!$G$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>N=100000</c:v>
+                  <c:v>N=1000000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1967,7 +2172,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Eficiência!$A$2:$A$4</c:f>
+              <c:f>'Dados gerais'!$A$12:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1984,18 +2189,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Eficiência!$G$2:$G$4</c:f>
+              <c:f>'Dados gerais'!$G$12:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.88554678235778</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.38000711063508</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20.6258325756713</c:v>
+                  <c:v>1.75115002399951</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.15722351692195</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.1942434666391</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2003,11 +2208,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="9391622"/>
-        <c:axId val="22017552"/>
+        <c:axId val="82973514"/>
+        <c:axId val="73200654"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="9391622"/>
+        <c:axId val="82973514"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2063,7 +2268,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22017552"/>
+        <c:crossAx val="73200654"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2071,7 +2276,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22017552"/>
+        <c:axId val="73200654"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2136,7 +2341,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9391622"/>
+        <c:crossAx val="82973514"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2188,16 +2393,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>48960</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>183240</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>793080</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>28440</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>115920</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>50040</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>151200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2205,8 +2410,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="48960" y="945360"/>
-        <a:ext cx="7390080" cy="4090680"/>
+        <a:off x="6455880" y="360"/>
+        <a:ext cx="5759640" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2216,23 +2421,18 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>232560</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>758160</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>103320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>427680</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>87840</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>15120</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2240,34 +2440,29 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="232560" y="1077120"/>
-        <a:ext cx="6697440" cy="3767040"/>
+        <a:off x="6420960" y="3192120"/>
+        <a:ext cx="5759640" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>106200</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>2160</xdr:rowOff>
+      <xdr:colOff>728640</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>810360</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>88200</xdr:rowOff>
+      <xdr:colOff>12600</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>112680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2275,12 +2470,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="106200" y="954720"/>
-        <a:ext cx="7206480" cy="4053600"/>
+        <a:off x="728640" y="3213000"/>
+        <a:ext cx="5759640" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2400,20 +2595,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="J41" activeCellId="0" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.15"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2429,355 +2622,321 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>10</v>
+        <v>0.00072044</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>0.00063971</v>
+        <v>0.00067737</v>
       </c>
       <c r="D2" s="1" t="n">
+        <v>0.00203937</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>0.01197194</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0.06476401</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>0.5710533</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>0.00057068</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>0.00057719</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0.00100679</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0.00694014</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0.03981932</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>0.33275941</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>0.0005289</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0.00047626</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0.00060595</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0.00245745</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0.01868315</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0.19386472</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <f aca="false">B2/B2</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="n">
         <f aca="false">C2/C2</f>
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="n">
-        <f aca="false">D2/C2</f>
-        <v>1563.20832877398</v>
+      <c r="D7" s="1" t="n">
+        <f aca="false">D2/D2</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <f aca="false">E2/E2</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <f aca="false">F2/F2</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <f aca="false">G2/G2</f>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <f aca="false">B2/B3</f>
+        <v>1.26242377514544</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <f aca="false">C2/C3</f>
+        <v>1.17356503057919</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <f aca="false">D2/D3</f>
+        <v>2.02561606690571</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <f aca="false">E2/E3</f>
+        <v>1.7250286017285</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <f aca="false">F2/F3</f>
+        <v>1.62644691069561</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <f aca="false">G2/G3</f>
+        <v>1.71611465472907</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <f aca="false">B2/B4</f>
+        <v>1.36214785403668</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <f aca="false">C2/C4</f>
+        <v>1.42226934867509</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <f aca="false">D2/D4</f>
+        <v>3.36557471738592</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <f aca="false">E2/E4</f>
+        <v>4.87169220126554</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <f aca="false">F2/F4</f>
+        <v>3.46643954579394</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <f aca="false">G2/G4</f>
+        <v>2.94562775527182</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>0.00075223</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <f aca="false">C3/C3</f>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="n">
-        <f aca="false">D3/C3</f>
-        <v>1329.3806415591</v>
+      <c r="B12" s="1" t="n">
+        <f aca="false">B7/B2</f>
+        <v>1388.04064182999</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <f aca="false">C7/C2</f>
+        <v>1476.29803504732</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <f aca="false">D7/D2</f>
+        <v>490.347509279827</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <f aca="false">E7/E2</f>
+        <v>83.5286511626353</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <f aca="false">F7/F2</f>
+        <v>15.4406745351315</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <f aca="false">G7/G2</f>
+        <v>1.75115002399951</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>0.00168294</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <f aca="false">C4/C4</f>
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <f aca="false">D4/C4</f>
-        <v>594.198248303564</v>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <f aca="false">B8/B3</f>
+        <v>2212.13950926165</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <f aca="false">C8/C3</f>
+        <v>2033.23867457715</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <f aca="false">D8/D3</f>
+        <v>2011.95489318101</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <f aca="false">E8/E3</f>
+        <v>248.558184954265</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <f aca="false">F8/F3</f>
+        <v>40.8456726708445</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <f aca="false">G8/G3</f>
+        <v>5.15722351692195</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>10000</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>0.01118532</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <f aca="false">C5/C5</f>
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <f aca="false">D5/C5</f>
-        <v>89.4028959386052</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>100000</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>0.06259119</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <f aca="false">C6/C6</f>
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <f aca="false">D6/C6</f>
-        <v>15.9766893711399</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>0.53035014</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <f aca="false">C7/C7</f>
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <f aca="false">D7/C7</f>
-        <v>1.88554678235778</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>0.00059671</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <f aca="false">C2/C8</f>
-        <v>1.07206180556719</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <f aca="false">D8/C8</f>
-        <v>1796.62114857668</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>0.00064081</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <f aca="false">C3/C9</f>
-        <v>1.17387369110969</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <f aca="false">D9/C9</f>
-        <v>1831.8591955645</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>0.00107316</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <f aca="false">C4/C10</f>
-        <v>1.56820977300682</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <f aca="false">D10/C10</f>
-        <v>1461.30099240264</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1" t="n">
-        <v>10000</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>0.00733196</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <f aca="false">C5/C11</f>
-        <v>1.52555660423679</v>
-      </c>
-      <c r="E11" s="1" t="n">
-        <f aca="false">D11/C11</f>
-        <v>208.069411758492</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1" t="n">
-        <v>100000</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>0.0389873</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <f aca="false">C6/C12</f>
-        <v>1.60542509996845</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <f aca="false">D12/C12</f>
-        <v>41.1781554498119</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>0.28831734</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <f aca="false">C7/C13</f>
-        <v>1.83946667931939</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <f aca="false">D13/C13</f>
-        <v>6.38000711063508</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="n">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>10</v>
+        <f aca="false">B9/B4</f>
+        <v>2575.43553419679</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>0.00053342</v>
+        <f aca="false">C9/C4</f>
+        <v>2986.32962809199</v>
       </c>
       <c r="D14" s="1" t="n">
-        <f aca="false">C2/C14</f>
-        <v>1.19926137002737</v>
+        <f aca="false">D9/D4</f>
+        <v>5554.21192736352</v>
       </c>
       <c r="E14" s="1" t="n">
-        <f aca="false">D14/C14</f>
-        <v>2248.24972822048</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>0.00056376</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <f aca="false">C3/C15</f>
-        <v>1.33430892578402</v>
-      </c>
-      <c r="E15" s="1" t="n">
-        <f aca="false">D15/C15</f>
-        <v>2366.80311796513</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>0.00067451</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <f aca="false">C4/C16</f>
-        <v>2.49505567004196</v>
-      </c>
-      <c r="E16" s="1" t="n">
-        <f aca="false">D16/C16</f>
-        <v>3699.06401690406</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="n">
-        <v>10000</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <v>0.003302</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <f aca="false">C5/C17</f>
-        <v>3.38743791641429</v>
-      </c>
-      <c r="E17" s="1" t="n">
-        <f aca="false">D17/C17</f>
-        <v>1025.87459612789</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1" t="n">
-        <v>100000</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>0.02230055</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <f aca="false">C6/C18</f>
-        <v>2.80671059682385</v>
-      </c>
-      <c r="E18" s="1" t="n">
-        <f aca="false">D18/C18</f>
-        <v>125.858357611083</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="C19" s="1" t="n">
-        <v>0.16035245</v>
-      </c>
-      <c r="D19" s="1" t="n">
-        <f aca="false">C7/C19</f>
-        <v>3.30740278679871</v>
-      </c>
-      <c r="E19" s="1" t="n">
-        <f aca="false">D19/C19</f>
-        <v>20.6258325756713</v>
+        <f aca="false">E9/E4</f>
+        <v>1982.41762854404</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <f aca="false">F9/F4</f>
+        <v>185.538281595659</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <f aca="false">G9/G4</f>
+        <v>15.1942434666391</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A14:A19"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2785,645 +2944,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H19"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="0" width="16.42"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>0.00063971</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>0.00075223</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>0.00168294</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>0.01118532</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>0.06259119</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>0.53035014</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>0.00059671</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>0.00064081</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>0.00107316</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>0.00733196</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>0.0389873</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>0.28831734</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>0.00053342</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>0.00056376</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>0.00067451</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>0.003302</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>0.02230055</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>0.16035245</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G19"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="n">
-        <v>1.072061806</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>1.173873691</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>1.568209773</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>1.525556604</v>
-      </c>
-      <c r="F3" s="3" t="n">
-        <v>1.6054251</v>
-      </c>
-      <c r="G3" s="3" t="n">
-        <v>1.839466679</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="n">
-        <v>1.19926137</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>1.334308926</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>2.49505567</v>
-      </c>
-      <c r="E4" s="3" t="n">
-        <v>3.387437916</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>2.806710597</v>
-      </c>
-      <c r="G4" s="3" t="n">
-        <v>3.307402787</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G19"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>1563.20832877398</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>1329.3806415591</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>594.198248303564</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>89.4028959386052</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>15.9766893711399</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>1.88554678235778</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>1796.62114857668</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>1831.8591955645</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>1461.30099240264</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>208.069411758492</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>41.1781554498119</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>6.38000711063508</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>2248.24972822048</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>2366.80311796513</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>3699.06401690406</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>1025.87459612789</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>125.858357611083</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>20.6258325756713</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
-  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FIX: Fixed the efficiency collumn on the Metricas.xlsx file
</commit_message>
<xml_diff>
--- a/Métricas.xlsx
+++ b/Métricas.xlsx
@@ -56,11 +56,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -79,11 +80,19 @@
     </font>
     <font>
       <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -130,12 +139,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -224,12 +237,20 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:rPr>
               <a:t>Threads X Tempo</a:t>
             </a:r>
@@ -280,11 +301,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -364,11 +390,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -448,11 +479,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -532,11 +568,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -616,11 +657,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -700,11 +746,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -756,11 +807,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="71560624"/>
-        <c:axId val="34231772"/>
+        <c:axId val="6540879"/>
+        <c:axId val="27708951"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="71560624"/>
+        <c:axId val="6540879"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -774,12 +825,20 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:rPr>
                   <a:t>Threads</a:t>
                 </a:r>
@@ -794,7 +853,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -811,12 +870,16 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34231772"/>
+        <c:crossAx val="27708951"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -824,7 +887,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34231772"/>
+        <c:axId val="27708951"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -847,12 +910,20 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:rPr>
                   <a:t>Tempo</a:t>
                 </a:r>
@@ -867,7 +938,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -884,12 +955,16 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71560624"/>
+        <c:crossAx val="6540879"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -917,7 +992,11 @@
         <a:p>
           <a:pPr>
             <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Arial"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:defRPr>
           </a:pPr>
         </a:p>
@@ -950,12 +1029,20 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:rPr>
               <a:t>Threads X Aceleração</a:t>
             </a:r>
@@ -1006,11 +1093,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1090,11 +1182,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1174,11 +1271,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1258,11 +1360,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1342,11 +1449,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1426,11 +1538,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1482,11 +1599,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="39911192"/>
-        <c:axId val="63862364"/>
+        <c:axId val="43169247"/>
+        <c:axId val="44029469"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39911192"/>
+        <c:axId val="43169247"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1500,12 +1617,20 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:rPr>
                   <a:t>Threads</a:t>
                 </a:r>
@@ -1520,7 +1645,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1537,12 +1662,16 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63862364"/>
+        <c:crossAx val="44029469"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1550,7 +1679,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63862364"/>
+        <c:axId val="44029469"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1573,12 +1702,20 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:rPr>
                   <a:t>Aceleração</a:t>
                 </a:r>
@@ -1593,7 +1730,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1610,12 +1747,16 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39911192"/>
+        <c:crossAx val="43169247"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1643,7 +1784,11 @@
         <a:p>
           <a:pPr>
             <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Arial"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:defRPr>
           </a:pPr>
         </a:p>
@@ -1676,12 +1821,20 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:rPr>
               <a:t>Threads X Eficiência</a:t>
             </a:r>
@@ -1732,11 +1885,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1774,13 +1932,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1388.04064182999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2212.13950926165</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2575.43553419679</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.63121188757272</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.34053696350917</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1816,11 +1974,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1858,13 +2021,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1476.29803504732</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2033.23867457715</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2986.32962809199</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.586782515289595</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.355567337168773</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1900,11 +2063,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1942,13 +2110,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>490.347509279827</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2011.95489318101</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5554.21192736352</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.01280803345286</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84139367934648</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1984,11 +2152,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2026,13 +2199,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>83.5286511626353</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>248.558184954265</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1982.41762854404</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.86251430086425</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.21792305031639</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2068,11 +2241,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2110,13 +2288,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15.4406745351315</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40.8456726708445</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>185.538281595659</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.813223455347805</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.866609886448485</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2152,11 +2330,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2194,13 +2377,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.75115002399951</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.15722351692195</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15.1942434666391</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.858057327364535</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.736406938817955</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2208,11 +2391,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="82973514"/>
-        <c:axId val="73200654"/>
+        <c:axId val="64018600"/>
+        <c:axId val="15729854"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82973514"/>
+        <c:axId val="64018600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2226,12 +2409,20 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:rPr>
                   <a:t>Threads</a:t>
                 </a:r>
@@ -2246,7 +2437,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2263,12 +2454,16 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73200654"/>
+        <c:crossAx val="15729854"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2276,7 +2471,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73200654"/>
+        <c:axId val="15729854"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2299,12 +2494,20 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:rPr>
                   <a:t>Eficiência</a:t>
                 </a:r>
@@ -2319,7 +2522,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2336,12 +2539,16 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82973514"/>
+        <c:crossAx val="64018600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2369,7 +2576,11 @@
         <a:p>
           <a:pPr>
             <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Arial"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:defRPr>
           </a:pPr>
         </a:p>
@@ -2400,9 +2611,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>50040</xdr:colOff>
+      <xdr:colOff>49680</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>151200</xdr:rowOff>
+      <xdr:rowOff>150840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2411,7 +2622,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="6455880" y="360"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:ext cx="5759280" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2430,9 +2641,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>15120</xdr:colOff>
+      <xdr:colOff>14760</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2441,7 +2652,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="6420960" y="3192120"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:ext cx="5759280" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2460,9 +2671,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>12600</xdr:colOff>
+      <xdr:colOff>12240</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2471,7 +2682,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="728640" y="3213000"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:ext cx="5759280" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2598,342 +2809,342 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J41" activeCellId="0" sqref="J41"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>0.00072044</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="2" t="n">
         <v>0.00067737</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="2" t="n">
         <v>0.00203937</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="2" t="n">
         <v>0.01197194</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="2" t="n">
         <v>0.06476401</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="G2" s="2" t="n">
         <v>0.5710533</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>0.00057068</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <v>0.00057719</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="2" t="n">
         <v>0.00100679</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>0.00694014</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="2" t="n">
         <v>0.03981932</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="G3" s="2" t="n">
         <v>0.33275941</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>0.0005289</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <v>0.00047626</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="2" t="n">
         <v>0.00060595</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="2" t="n">
         <v>0.00245745</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="2" t="n">
         <v>0.01868315</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="G4" s="2" t="n">
         <v>0.19386472</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="2" t="n">
         <f aca="false">B2/B2</f>
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="2" t="n">
         <f aca="false">C2/C2</f>
         <v>1</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="2" t="n">
         <f aca="false">D2/D2</f>
         <v>1</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="2" t="n">
         <f aca="false">E2/E2</f>
         <v>1</v>
       </c>
-      <c r="F7" s="1" t="n">
+      <c r="F7" s="2" t="n">
         <f aca="false">F2/F2</f>
         <v>1</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="G7" s="2" t="n">
         <f aca="false">G2/G2</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="2" t="n">
         <f aca="false">B2/B3</f>
         <v>1.26242377514544</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="2" t="n">
         <f aca="false">C2/C3</f>
         <v>1.17356503057919</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="2" t="n">
         <f aca="false">D2/D3</f>
         <v>2.02561606690571</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="2" t="n">
         <f aca="false">E2/E3</f>
         <v>1.7250286017285</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="F8" s="2" t="n">
         <f aca="false">F2/F3</f>
         <v>1.62644691069561</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="2" t="n">
         <f aca="false">G2/G3</f>
         <v>1.71611465472907</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="2" t="n">
         <f aca="false">B2/B4</f>
         <v>1.36214785403668</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="2" t="n">
         <f aca="false">C2/C4</f>
         <v>1.42226934867509</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="2" t="n">
         <f aca="false">D2/D4</f>
         <v>3.36557471738592</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="2" t="n">
         <f aca="false">E2/E4</f>
         <v>4.87169220126554</v>
       </c>
-      <c r="F9" s="1" t="n">
+      <c r="F9" s="2" t="n">
         <f aca="false">F2/F4</f>
         <v>3.46643954579394</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="G9" s="2" t="n">
         <f aca="false">G2/G4</f>
         <v>2.94562775527182</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B12" s="1" t="n">
-        <f aca="false">B7/B2</f>
-        <v>1388.04064182999</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <f aca="false">C7/C2</f>
-        <v>1476.29803504732</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <f aca="false">D7/D2</f>
-        <v>490.347509279827</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <f aca="false">E7/E2</f>
-        <v>83.5286511626353</v>
-      </c>
-      <c r="F12" s="1" t="n">
-        <f aca="false">F7/F2</f>
-        <v>15.4406745351315</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <f aca="false">G7/G2</f>
-        <v>1.75115002399951</v>
+      <c r="B12" s="2" t="n">
+        <f aca="false">B7/A12</f>
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <f aca="false">C7/B12</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <f aca="false">D7/C12</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <f aca="false">E7/D12</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <f aca="false">F7/E12</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <f aca="false">G7/F12</f>
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B13" s="1" t="n">
-        <f aca="false">B8/B3</f>
-        <v>2212.13950926165</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <f aca="false">C8/C3</f>
-        <v>2033.23867457715</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <f aca="false">D8/D3</f>
-        <v>2011.95489318101</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <f aca="false">E8/E3</f>
-        <v>248.558184954265</v>
-      </c>
-      <c r="F13" s="1" t="n">
-        <f aca="false">F8/F3</f>
-        <v>40.8456726708445</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <f aca="false">G8/G3</f>
-        <v>5.15722351692195</v>
+      <c r="B13" s="2" t="n">
+        <f aca="false">B8/A13</f>
+        <v>0.63121188757272</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <f aca="false">C8/A13</f>
+        <v>0.586782515289595</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <f aca="false">D8/A13</f>
+        <v>1.01280803345286</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <f aca="false">E8/A13</f>
+        <v>0.86251430086425</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <f aca="false">F8/A13</f>
+        <v>0.813223455347805</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <f aca="false">G8/A13</f>
+        <v>0.858057327364535</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B14" s="1" t="n">
-        <f aca="false">B9/B4</f>
-        <v>2575.43553419679</v>
-      </c>
-      <c r="C14" s="1" t="n">
-        <f aca="false">C9/C4</f>
-        <v>2986.32962809199</v>
-      </c>
-      <c r="D14" s="1" t="n">
-        <f aca="false">D9/D4</f>
-        <v>5554.21192736352</v>
-      </c>
-      <c r="E14" s="1" t="n">
-        <f aca="false">E9/E4</f>
-        <v>1982.41762854404</v>
-      </c>
-      <c r="F14" s="1" t="n">
-        <f aca="false">F9/F4</f>
-        <v>185.538281595659</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <f aca="false">G9/G4</f>
-        <v>15.1942434666391</v>
+      <c r="B14" s="2" t="n">
+        <f aca="false">B9/A14</f>
+        <v>0.34053696350917</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <f aca="false">C9/A14</f>
+        <v>0.355567337168773</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <f aca="false">D9/A14</f>
+        <v>0.84139367934648</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <f aca="false">E9/A14</f>
+        <v>1.21792305031639</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <f aca="false">F9/A14</f>
+        <v>0.866609886448485</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <f aca="false">G9/A14</f>
+        <v>0.736406938817955</v>
       </c>
     </row>
   </sheetData>

</xml_diff>